<commit_message>
DRE, Cronograma e Estimativa de Tamanho
</commit_message>
<xml_diff>
--- a/Estimativa de Tamanho.xlsx
+++ b/Estimativa de Tamanho.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f6l6p\Documents\GitHub\Engenharia-de-Software\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A5A0D4AB-6F23-440B-ABCC-FC9D54E8662E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -28,7 +34,7 @@
     <definedName name="TotalHorasProjeto">Geral!#REF!</definedName>
     <definedName name="UC">'RFS ou RFC'!$A$12:$C$38</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -38,12 +44,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -126,12 +132,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -209,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="212">
   <si>
     <t>Projeto:</t>
   </si>
@@ -254,9 +260,6 @@
     <t>Data:</t>
   </si>
   <si>
-    <t>30/05/2018</t>
-  </si>
-  <si>
     <t>Vs. do Documento:</t>
   </si>
   <si>
@@ -872,19 +875,19 @@
     <t>Barbearia Bom Bigode - Sistema de Barbearia</t>
   </si>
   <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>Estimativa de Esforço de Projeto baseado em                                                                Pontos de Caso de Uso (vs 1.2)</t>
-  </si>
-  <si>
     <t>Fase de Desenvolvimento Implementação</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Estimativa de Esforço de Projeto baseado em                                                                Pontos de Caso de Uso (vs 2.0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1895,48 +1898,6 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1954,6 +1915,48 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1965,19 +1968,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2021,7 +2024,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2072,7 +2081,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2123,7 +2138,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2174,7 +2195,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2217,7 +2244,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2260,7 +2293,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2308,7 +2347,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2359,7 +2404,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2410,7 +2461,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2461,7 +2518,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2512,7 +2575,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2056" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="2056" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2555,7 +2624,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2054" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="2054" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2598,7 +2673,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2052" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="2052" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2641,7 +2722,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2050" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="2050" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2927,21 +3014,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2987,32 +3074,32 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="107" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
       <c r="K3" s="2"/>
       <c r="L3"/>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
       <c r="K4" s="2"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -3032,54 +3119,54 @@
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="123" t="s">
-        <v>209</v>
-      </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="125" t="s">
+      <c r="C7" s="110"/>
+      <c r="D7" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="112"/>
+      <c r="D8" s="3">
+        <v>43269</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="117" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="117"/>
+      <c r="G8" s="113"/>
       <c r="H8" s="5" t="s">
         <v>210</v>
       </c>
@@ -3092,14 +3179,14 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
+      <c r="D9" s="114" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
       <c r="J9" s="8"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -3134,43 +3221,43 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12"/>
+      <c r="G12" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12"/>
-      <c r="G12" s="120" t="s">
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="9" t="s">
+      <c r="K12" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>10</v>
       </c>
       <c r="L12"/>
       <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="113" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
+      <c r="B13" s="117" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
       <c r="E13" s="11">
         <f>(Atores!D10+'RFS ou RFC'!D10)*Fatores!E22*Fatores!G36</f>
         <v>93.879099999999994</v>
       </c>
       <c r="F13"/>
-      <c r="G13" s="113" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
+      <c r="G13" s="117" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
       <c r="J13" s="12">
         <f t="shared" ref="J13:J20" si="0">$E$13*$E$14*K13</f>
         <v>23.939170499999999</v>
@@ -3182,20 +3269,20 @@
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="114" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
+      <c r="B14" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
       <c r="E14" s="15">
         <v>3</v>
       </c>
       <c r="F14"/>
-      <c r="G14" s="112" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="112"/>
-      <c r="I14" s="112"/>
+      <c r="G14" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="119"/>
+      <c r="I14" s="119"/>
       <c r="J14" s="16">
         <f t="shared" si="0"/>
         <v>43.653781499999994</v>
@@ -3207,16 +3294,16 @@
       <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="115"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="115"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15" s="112" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="112"/>
-      <c r="I15" s="112"/>
+      <c r="G15" s="119" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
       <c r="J15" s="16">
         <f t="shared" si="0"/>
         <v>16.898237999999999</v>
@@ -3228,16 +3315,16 @@
       <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="111"/>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="112" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="112"/>
-      <c r="I16" s="112"/>
+      <c r="G16" s="119" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
       <c r="J16" s="16">
         <f t="shared" si="0"/>
         <v>16.5669</v>
@@ -3255,11 +3342,11 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="107" t="s">
-        <v>212</v>
-      </c>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
+      <c r="G17" s="122" t="s">
+        <v>209</v>
+      </c>
+      <c r="H17" s="122"/>
+      <c r="I17" s="122"/>
       <c r="J17" s="16">
         <f t="shared" si="0"/>
         <v>142.47533999999999</v>
@@ -3277,11 +3364,11 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
+      <c r="G18" s="122" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="122"/>
+      <c r="I18" s="122"/>
       <c r="J18" s="16">
         <f t="shared" si="0"/>
         <v>6.6267599999999991</v>
@@ -3298,11 +3385,11 @@
       <c r="D19"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="107"/>
-      <c r="I19" s="107"/>
+      <c r="G19" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="122"/>
+      <c r="I19" s="122"/>
       <c r="J19" s="16">
         <f t="shared" si="0"/>
         <v>18.223590000000002</v>
@@ -3315,17 +3402,17 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="107" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
+      <c r="G20" s="122" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="122"/>
+      <c r="I20" s="122"/>
       <c r="J20" s="16">
         <f t="shared" si="0"/>
         <v>13.253519999999998</v>
@@ -3342,11 +3429,11 @@
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="108" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
+      <c r="G21" s="123" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
       <c r="J21" s="20">
         <f>SUM(J13:J20)</f>
         <v>281.63729999999998</v>
@@ -3358,36 +3445,36 @@
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="124" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="124"/>
+      <c r="D22" s="124"/>
+      <c r="E22" s="124"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="124"/>
+      <c r="H22" s="124"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="124"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
-      <c r="L22" s="14"/>
-    </row>
-    <row r="23" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="110" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
+      <c r="C23" s="125"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="125"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="125"/>
+      <c r="H23" s="125"/>
+      <c r="I23" s="125"/>
+      <c r="J23" s="125"/>
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -3401,7 +3488,7 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -3427,7 +3514,7 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -3440,47 +3527,47 @@
       <c r="L27" s="14"/>
     </row>
     <row r="28" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="110" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="110"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
-      <c r="G28" s="110"/>
-      <c r="H28" s="110"/>
-      <c r="I28" s="110"/>
-      <c r="J28" s="110"/>
+      <c r="B28" s="125" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="125"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="125"/>
+      <c r="F28" s="125"/>
+      <c r="G28" s="125"/>
+      <c r="H28" s="125"/>
+      <c r="I28" s="125"/>
+      <c r="J28" s="125"/>
     </row>
     <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3488,7 +3575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -3527,7 +3614,7 @@
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="126" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="126"/>
       <c r="D2" s="126"/>
@@ -3585,13 +3672,13 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="D6" s="27" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>31</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
@@ -3605,7 +3692,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="29">
         <v>1</v>
@@ -3626,7 +3713,7 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="32">
         <v>2</v>
@@ -3647,7 +3734,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="35">
         <v>3</v>
@@ -3669,7 +3756,7 @@
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="38">
         <f>(C7*D7)+(C8*D8)+(C9*D9)</f>
@@ -3704,31 +3791,31 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="39" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="42">
         <f>D10</f>
@@ -3740,7 +3827,7 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14:C15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14:C15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Simples,Médio,Complexo"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3753,7 +3840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -3792,7 +3879,7 @@
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="127" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="127"/>
       <c r="D2" s="127"/>
@@ -3835,13 +3922,13 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="47" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>43</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6"/>
@@ -3851,7 +3938,7 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7" s="49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="50">
         <v>3</v>
@@ -3868,7 +3955,7 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="53">
         <v>4</v>
@@ -3885,7 +3972,7 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" s="55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="56">
         <v>5</v>
@@ -3903,7 +3990,7 @@
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="58">
         <f>(C7*D7)+(C8*D8)+(C9*D9)</f>
@@ -3926,19 +4013,19 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="C12" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="D12" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="62" t="s">
         <v>47</v>
-      </c>
-      <c r="D12" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>48</v>
       </c>
       <c r="F12"/>
       <c r="H12"/>
@@ -3946,19 +4033,19 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="63" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B13" s="64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="65">
         <v>1</v>
       </c>
       <c r="D13" s="66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13"/>
       <c r="H13"/>
@@ -3968,10 +4055,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="65">
         <v>1</v>
@@ -3981,7 +4068,7 @@
         <v>Simples</v>
       </c>
       <c r="E14" s="64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14"/>
       <c r="H14"/>
@@ -3991,10 +4078,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="63" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="65">
         <v>1</v>
@@ -4004,7 +4091,7 @@
         <v>Simples</v>
       </c>
       <c r="E15" s="64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15"/>
       <c r="H15"/>
@@ -4012,10 +4099,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16" s="64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" s="65">
         <v>2</v>
@@ -4025,7 +4112,7 @@
         <v>Médio</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16"/>
       <c r="H16"/>
@@ -4035,10 +4122,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17" s="65">
         <v>1</v>
@@ -4048,7 +4135,7 @@
         <v>Simples</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F17"/>
       <c r="H17"/>
@@ -4058,10 +4145,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" s="65">
         <v>1</v>
@@ -4071,7 +4158,7 @@
         <v>Simples</v>
       </c>
       <c r="E18" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F18"/>
       <c r="H18"/>
@@ -4079,10 +4166,10 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19" s="64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="65">
         <v>1</v>
@@ -4092,7 +4179,7 @@
         <v>Simples</v>
       </c>
       <c r="E19" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F19"/>
       <c r="H19" s="43"/>
@@ -4102,10 +4189,10 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="65">
         <v>1</v>
@@ -4115,7 +4202,7 @@
         <v>Simples</v>
       </c>
       <c r="E20" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F20"/>
       <c r="H20" s="43"/>
@@ -4125,10 +4212,10 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B21" s="64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C21" s="65">
         <v>1</v>
@@ -4138,7 +4225,7 @@
         <v>Simples</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21"/>
       <c r="H21" s="43"/>
@@ -4148,10 +4235,10 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="65">
         <v>1</v>
@@ -4161,7 +4248,7 @@
         <v>Simples</v>
       </c>
       <c r="E22" s="64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22"/>
       <c r="H22" s="43"/>
@@ -4171,10 +4258,10 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B23" s="64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C23" s="65">
         <v>1</v>
@@ -4184,7 +4271,7 @@
         <v>Simples</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23"/>
       <c r="H23" s="43"/>
@@ -4194,10 +4281,10 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24" s="64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="65">
         <v>2</v>
@@ -4207,7 +4294,7 @@
         <v>Médio</v>
       </c>
       <c r="E24" s="64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F24"/>
       <c r="O24" s="67">
@@ -4216,10 +4303,10 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" s="64" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25" s="65">
         <v>1</v>
@@ -4229,7 +4316,7 @@
         <v>Simples</v>
       </c>
       <c r="E25" s="64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25"/>
       <c r="O25" s="67">
@@ -4238,10 +4325,10 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C26" s="65">
         <v>1</v>
@@ -4251,7 +4338,7 @@
         <v>Simples</v>
       </c>
       <c r="E26" s="64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F26"/>
       <c r="O26" s="67">
@@ -4260,10 +4347,10 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27" s="64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" s="65">
         <v>1</v>
@@ -4273,7 +4360,7 @@
         <v>Simples</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F27"/>
       <c r="O27" s="67">
@@ -4282,10 +4369,10 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" s="64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" s="65">
         <v>1</v>
@@ -4295,7 +4382,7 @@
         <v>Simples</v>
       </c>
       <c r="E28" s="64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28"/>
       <c r="O28" s="67">
@@ -4304,10 +4391,10 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C29" s="65">
         <v>3</v>
@@ -4317,7 +4404,7 @@
         <v>Complexo</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F29"/>
       <c r="O29" s="67">
@@ -4326,10 +4413,10 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B30" s="68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C30" s="65">
         <v>2</v>
@@ -4339,7 +4426,7 @@
         <v>Médio</v>
       </c>
       <c r="E30" s="64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30"/>
       <c r="O30" s="67">
@@ -4348,10 +4435,10 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B31" s="64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" s="65">
         <v>1</v>
@@ -4361,7 +4448,7 @@
         <v>Simples</v>
       </c>
       <c r="E31" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F31"/>
       <c r="O31" s="67">
@@ -4370,10 +4457,10 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" s="64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C32" s="65">
         <v>1</v>
@@ -4383,7 +4470,7 @@
         <v>Simples</v>
       </c>
       <c r="E32" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F32"/>
       <c r="O32" s="67">
@@ -4392,10 +4479,10 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C33" s="69">
         <v>2</v>
@@ -4405,10 +4492,10 @@
         <v>Médio</v>
       </c>
       <c r="E33" s="70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O33" s="67">
         <v>22</v>
@@ -4416,10 +4503,10 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B34" s="68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" s="65">
         <v>1</v>
@@ -4429,7 +4516,7 @@
         <v>Simples</v>
       </c>
       <c r="E34" s="70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O34" s="67">
         <v>23</v>
@@ -4437,10 +4524,10 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B35" s="64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C35" s="65">
         <v>1</v>
@@ -4450,7 +4537,7 @@
         <v>Simples</v>
       </c>
       <c r="E35" s="70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O35" s="67">
         <v>24</v>
@@ -4458,10 +4545,10 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" s="64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="65">
         <v>1</v>
@@ -4471,7 +4558,7 @@
         <v>Simples</v>
       </c>
       <c r="E36" s="70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O36" s="67">
         <v>25</v>
@@ -4479,10 +4566,10 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" s="64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C37" s="65">
         <v>3</v>
@@ -4492,7 +4579,7 @@
         <v>Complexo</v>
       </c>
       <c r="E37" s="64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O37" s="67">
         <v>26</v>
@@ -4500,10 +4587,10 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B38" s="68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C38" s="65">
         <v>3</v>
@@ -4513,7 +4600,7 @@
         <v>Complexo</v>
       </c>
       <c r="E38" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O38" s="67">
         <v>27</v>
@@ -4521,10 +4608,10 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B39" s="64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" s="65">
         <v>3</v>
@@ -4534,7 +4621,7 @@
         <v>Complexo</v>
       </c>
       <c r="E39" s="64" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O39" s="67">
         <v>28</v>
@@ -4542,10 +4629,10 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="63" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B40" s="64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C40" s="65">
         <v>3</v>
@@ -4555,7 +4642,7 @@
         <v>Complexo</v>
       </c>
       <c r="E40" s="64" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O40" s="67">
         <v>29</v>
@@ -4563,10 +4650,10 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41" s="64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" s="65">
         <v>2</v>
@@ -4576,7 +4663,7 @@
         <v>Médio</v>
       </c>
       <c r="E41" s="64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O41" s="67">
         <v>30</v>
@@ -4584,10 +4671,10 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B42" s="68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C42" s="65">
         <v>1</v>
@@ -4597,7 +4684,7 @@
         <v>Simples</v>
       </c>
       <c r="E42" s="64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O42" s="67">
         <v>31</v>
@@ -4605,10 +4692,10 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B43" s="64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C43" s="65">
         <v>1</v>
@@ -4618,7 +4705,7 @@
         <v>Simples</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O43" s="67">
         <v>32</v>
@@ -4626,10 +4713,10 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="63" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B44" s="64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C44" s="65">
         <v>2</v>
@@ -4639,7 +4726,7 @@
         <v>Médio</v>
       </c>
       <c r="E44" s="64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O44" s="67">
         <v>33</v>
@@ -4647,10 +4734,10 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="64" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C45" s="65">
         <v>3</v>
@@ -4660,7 +4747,7 @@
         <v>Complexo</v>
       </c>
       <c r="E45" s="64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O45" s="67">
         <v>34</v>
@@ -4668,10 +4755,10 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C46" s="65">
         <v>3</v>
@@ -4681,7 +4768,7 @@
         <v>Complexo</v>
       </c>
       <c r="E46" s="64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O46" s="67">
         <v>35</v>
@@ -4689,10 +4776,10 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="64" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C47" s="65">
         <v>3</v>
@@ -4702,7 +4789,7 @@
         <v>Complexo</v>
       </c>
       <c r="E47" s="64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O47" s="67">
         <v>36</v>
@@ -4710,10 +4797,10 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" s="64" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C48" s="65">
         <v>2</v>
@@ -4723,7 +4810,7 @@
         <v>Médio</v>
       </c>
       <c r="E48" s="64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O48" s="67">
         <v>37</v>
@@ -9535,25 +9622,25 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A12:E48"/>
+  <autoFilter ref="A12:E48" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="2">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" sqref="B13 B27:B29 B23:B25 B15:B17 B19:B21 B31:B33 B35:B37 B39:B41 B43:B48">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" sqref="B13 B27:B29 B23:B25 B15:B17 B19:B21 B31:B33 B35:B37 B39:B41 B43:B48" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D32 D34:D48">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D32 D34:D48" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>$B$7:$B$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C13:C32 C34:C48">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C13:C32 C34:C48" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9566,7 +9653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK36"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -9628,7 +9715,7 @@
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="126" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="126"/>
       <c r="D4" s="126"/>
@@ -9671,12 +9758,12 @@
       <c r="M6"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="131" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
+      <c r="B7" s="129" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="14"/>
@@ -9688,16 +9775,16 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" s="71" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="72" t="s">
         <v>64</v>
-      </c>
-      <c r="D8" s="72" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>65</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -9710,10 +9797,10 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="73" t="s">
         <v>66</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>67</v>
       </c>
       <c r="D9" s="32">
         <v>2</v>
@@ -9732,10 +9819,10 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="73" t="s">
         <v>68</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>69</v>
       </c>
       <c r="D10" s="32">
         <v>1</v>
@@ -9754,10 +9841,10 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="73" t="s">
         <v>70</v>
-      </c>
-      <c r="C11" s="73" t="s">
-        <v>71</v>
       </c>
       <c r="D11" s="32">
         <v>1</v>
@@ -9776,10 +9863,10 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="73" t="s">
         <v>72</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>73</v>
       </c>
       <c r="D12" s="32">
         <v>1</v>
@@ -9798,10 +9885,10 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="73" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>75</v>
       </c>
       <c r="D13" s="32">
         <v>1</v>
@@ -9820,10 +9907,10 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="73" t="s">
         <v>76</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>77</v>
       </c>
       <c r="D14" s="32">
         <v>0.5</v>
@@ -9842,10 +9929,10 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="73" t="s">
         <v>78</v>
-      </c>
-      <c r="C15" s="73" t="s">
-        <v>79</v>
       </c>
       <c r="D15" s="32">
         <v>0.5</v>
@@ -9864,10 +9951,10 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="73" t="s">
         <v>80</v>
-      </c>
-      <c r="C16" s="73" t="s">
-        <v>81</v>
       </c>
       <c r="D16" s="32">
         <v>2</v>
@@ -9886,10 +9973,10 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="73" t="s">
         <v>82</v>
-      </c>
-      <c r="C17" s="73" t="s">
-        <v>83</v>
       </c>
       <c r="D17" s="32">
         <v>1</v>
@@ -9908,10 +9995,10 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="73" t="s">
         <v>84</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>85</v>
       </c>
       <c r="D18" s="32">
         <v>1</v>
@@ -9930,10 +10017,10 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="73" t="s">
         <v>86</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>87</v>
       </c>
       <c r="D19" s="32">
         <v>1</v>
@@ -9952,10 +10039,10 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="73" t="s">
         <v>88</v>
-      </c>
-      <c r="C20" s="73" t="s">
-        <v>89</v>
       </c>
       <c r="D20" s="32">
         <v>1</v>
@@ -9974,10 +10061,10 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="73" t="s">
         <v>90</v>
-      </c>
-      <c r="C21" s="73" t="s">
-        <v>91</v>
       </c>
       <c r="D21" s="32">
         <v>1</v>
@@ -9996,7 +10083,7 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="130" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="130"/>
       <c r="D22" s="130"/>
@@ -10046,42 +10133,42 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="132" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
+      <c r="B26" s="131" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="131"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
       <c r="F26" s="76"/>
       <c r="G26" s="77"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="133" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="132" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="78" t="s">
         <v>64</v>
-      </c>
-      <c r="D27" s="133"/>
-      <c r="E27" s="133"/>
-      <c r="F27" s="78" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="78" t="s">
-        <v>65</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="129" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="129"/>
-      <c r="E28" s="129"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="133"/>
       <c r="F28" s="32">
         <v>1.5</v>
       </c>
@@ -10092,13 +10179,13 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="129" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="129"/>
-      <c r="E29" s="129"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="133"/>
       <c r="F29" s="32">
         <v>0.5</v>
       </c>
@@ -10109,13 +10196,13 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="133" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="129" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="129"/>
-      <c r="E30" s="129"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="133"/>
       <c r="F30" s="32">
         <v>1</v>
       </c>
@@ -10126,13 +10213,13 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="129" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="129"/>
-      <c r="E31" s="129"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
       <c r="F31" s="32">
         <v>0.5</v>
       </c>
@@ -10143,13 +10230,13 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="133" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="129" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="129"/>
-      <c r="E32" s="129"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="133"/>
       <c r="F32" s="32">
         <v>1</v>
       </c>
@@ -10160,13 +10247,13 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="133" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="129" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="129"/>
-      <c r="E33" s="129"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="133"/>
       <c r="F33" s="32">
         <v>2</v>
       </c>
@@ -10177,13 +10264,13 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="133" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="129" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="129"/>
-      <c r="E34" s="129"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="133"/>
       <c r="F34" s="32">
         <v>-1</v>
       </c>
@@ -10194,13 +10281,13 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="133" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="129" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="129"/>
-      <c r="E35" s="129"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
       <c r="F35" s="32">
         <v>-1</v>
       </c>
@@ -10211,7 +10298,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="130" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" s="130"/>
       <c r="D36" s="130"/>
@@ -10226,11 +10313,6 @@
   </sheetData>
   <sheetProtection password="C6D5" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="14">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
@@ -10240,13 +10322,18 @@
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21">
+    <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G28:G35 I28:I35">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G28:G35 I28:I35" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
@@ -10257,7 +10344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -10281,7 +10368,7 @@
     <row r="1" spans="1:55" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="80"/>
       <c r="B1" s="134" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C1" s="134"/>
       <c r="D1" s="134"/>
@@ -10511,37 +10598,37 @@
     <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" s="80"/>
       <c r="B5" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="D5" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="E5" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="84" t="s">
+      <c r="F5" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="84" t="s">
+      <c r="G5" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="G5" s="84" t="s">
+      <c r="H5" s="84" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="84" t="s">
+      <c r="I5" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="J5" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="J5" s="84" t="s">
+      <c r="K5" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="K5" s="84" t="s">
+      <c r="L5" s="85" t="s">
         <v>121</v>
-      </c>
-      <c r="L5" s="85" t="s">
-        <v>122</v>
       </c>
       <c r="M5" s="80"/>
       <c r="N5" s="80"/>
@@ -10590,7 +10677,7 @@
     <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6" s="80"/>
       <c r="B6" s="86" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="87">
         <v>150</v>
@@ -10671,7 +10758,7 @@
     <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7" s="80"/>
       <c r="B7" s="86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="88">
         <v>130</v>
@@ -11835,7 +11922,7 @@
     <row r="27" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A27" s="80"/>
       <c r="B27" s="98" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" s="99"/>
       <c r="D27" s="99">
@@ -11926,7 +12013,7 @@
       <c r="H28" s="80"/>
       <c r="I28" s="80"/>
       <c r="J28" s="135" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K28" s="135"/>
       <c r="L28" s="101">
@@ -11979,7 +12066,7 @@
     <row r="29" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A29" s="80"/>
       <c r="B29" s="102" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" s="103"/>
       <c r="D29" s="104"/>

</xml_diff>

<commit_message>
Atualização Est de Tam
</commit_message>
<xml_diff>
--- a/Estimativa de Tamanho.xlsx
+++ b/Estimativa de Tamanho.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ygor Salles\Documents\GitHub\Engenharia-de-Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f6l6p\Documents\GitHub\Engenharia-de-Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{82867DB5-2E13-401E-9F4E-EB61065BAD67}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -43,12 +44,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -100,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -131,12 +132,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -880,13 +881,13 @@
     <t>Estimativa de Esforço de Projeto baseado em                                                                Pontos de Caso de Uso (vs 2.0)</t>
   </si>
   <si>
-    <t>Ygor Salles, Igor, Bruno, Matheus, Felipe</t>
+    <t>Ygor Salles, Igor, Bruno, Matheus, Felipe Dias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1897,48 +1898,6 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1956,6 +1915,48 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1967,19 +1968,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3020,7 +3021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -3073,32 +3074,32 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="107" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
       <c r="K3" s="2"/>
       <c r="L3"/>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
       <c r="K4" s="2"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -3118,54 +3119,54 @@
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="123" t="s">
+      <c r="C6" s="108"/>
+      <c r="D6" s="109" t="s">
         <v>207</v>
       </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="125" t="s">
+      <c r="C7" s="110"/>
+      <c r="D7" s="111" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="116"/>
+      <c r="C8" s="112"/>
       <c r="D8" s="3">
         <v>43269</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="117" t="s">
+      <c r="F8" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="117"/>
+      <c r="G8" s="113"/>
       <c r="H8" s="5" t="s">
         <v>209</v>
       </c>
@@ -3178,14 +3179,14 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
       <c r="J9" s="8"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -3220,18 +3221,18 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
       <c r="F12"/>
-      <c r="G12" s="120" t="s">
+      <c r="G12" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
       <c r="J12" s="9" t="s">
         <v>7</v>
       </c>
@@ -3242,21 +3243,21 @@
       <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
       <c r="E13" s="11">
         <f>(Atores!D10+'RFS ou RFC'!D10)*Fatores!E22*Fatores!G36</f>
         <v>93.879099999999994</v>
       </c>
       <c r="F13"/>
-      <c r="G13" s="113" t="s">
+      <c r="G13" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
       <c r="J13" s="12">
         <f t="shared" ref="J13:J20" si="0">$E$13*$E$14*K13</f>
         <v>23.939170499999999</v>
@@ -3268,20 +3269,20 @@
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="114" t="s">
+      <c r="B14" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
       <c r="E14" s="15">
         <v>3</v>
       </c>
       <c r="F14"/>
-      <c r="G14" s="112" t="s">
+      <c r="G14" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="112"/>
-      <c r="I14" s="112"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="119"/>
       <c r="J14" s="16">
         <f t="shared" si="0"/>
         <v>43.653781499999994</v>
@@ -3293,16 +3294,16 @@
       <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="115"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="115"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15" s="112" t="s">
+      <c r="G15" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="112"/>
-      <c r="I15" s="112"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
       <c r="J15" s="16">
         <f t="shared" si="0"/>
         <v>16.898237999999999</v>
@@ -3314,16 +3315,16 @@
       <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="111"/>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="112" t="s">
+      <c r="G16" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="112"/>
-      <c r="I16" s="112"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
       <c r="J16" s="16">
         <f t="shared" si="0"/>
         <v>16.5669</v>
@@ -3341,11 +3342,11 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="107" t="s">
+      <c r="G17" s="122" t="s">
         <v>208</v>
       </c>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
+      <c r="H17" s="122"/>
+      <c r="I17" s="122"/>
       <c r="J17" s="16">
         <f t="shared" si="0"/>
         <v>142.47533999999999</v>
@@ -3363,11 +3364,11 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="107" t="s">
+      <c r="G18" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
+      <c r="H18" s="122"/>
+      <c r="I18" s="122"/>
       <c r="J18" s="16">
         <f t="shared" si="0"/>
         <v>6.6267599999999991</v>
@@ -3384,11 +3385,11 @@
       <c r="D19"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="107" t="s">
+      <c r="G19" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="107"/>
-      <c r="I19" s="107"/>
+      <c r="H19" s="122"/>
+      <c r="I19" s="122"/>
       <c r="J19" s="16">
         <f t="shared" si="0"/>
         <v>18.223590000000002</v>
@@ -3407,11 +3408,11 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="107" t="s">
+      <c r="G20" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
+      <c r="H20" s="122"/>
+      <c r="I20" s="122"/>
       <c r="J20" s="16">
         <f t="shared" si="0"/>
         <v>13.253519999999998</v>
@@ -3428,11 +3429,11 @@
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="108" t="s">
+      <c r="G21" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
       <c r="J21" s="20">
         <f>SUM(J13:J20)</f>
         <v>281.63729999999998</v>
@@ -3444,31 +3445,31 @@
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
+      <c r="C22" s="124"/>
+      <c r="D22" s="124"/>
+      <c r="E22" s="124"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="124"/>
+      <c r="H22" s="124"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="124"/>
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="110" t="s">
+      <c r="B23" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
+      <c r="C23" s="125"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="125"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="125"/>
+      <c r="H23" s="125"/>
+      <c r="I23" s="125"/>
+      <c r="J23" s="125"/>
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
@@ -3526,47 +3527,47 @@
       <c r="L27" s="14"/>
     </row>
     <row r="28" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="110" t="s">
+      <c r="B28" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="110"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
-      <c r="G28" s="110"/>
-      <c r="H28" s="110"/>
-      <c r="I28" s="110"/>
-      <c r="J28" s="110"/>
+      <c r="C28" s="125"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="125"/>
+      <c r="F28" s="125"/>
+      <c r="G28" s="125"/>
+      <c r="H28" s="125"/>
+      <c r="I28" s="125"/>
+      <c r="J28" s="125"/>
     </row>
     <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3574,7 +3575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -3826,7 +3827,7 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14:C15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14:C15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Simples,Médio,Complexo"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3839,7 +3840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -9621,25 +9622,25 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A12:E48"/>
+  <autoFilter ref="A12:E48" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="2">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" sqref="B13 B27:B29 B23:B25 B15:B17 B19:B21 B31:B33 B35:B37 B39:B41 B43:B48">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" sqref="B13 B27:B29 B23:B25 B15:B17 B19:B21 B31:B33 B35:B37 B39:B41 B43:B48" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D32 D34:D48">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D32 D34:D48" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>$B$7:$B$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C13:C32 C34:C48">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C13:C32 C34:C48" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9652,7 +9653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK36"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -9757,12 +9758,12 @@
       <c r="M6"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="129" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="14"/>
@@ -10132,12 +10133,12 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="132" t="s">
+      <c r="B26" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
+      <c r="C26" s="131"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
       <c r="F26" s="76"/>
       <c r="G26" s="77"/>
       <c r="I26"/>
@@ -10146,11 +10147,11 @@
       <c r="B27" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="133" t="s">
+      <c r="C27" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="133"/>
-      <c r="E27" s="133"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
       <c r="F27" s="78" t="s">
         <v>28</v>
       </c>
@@ -10163,11 +10164,11 @@
       <c r="B28" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="129" t="s">
+      <c r="C28" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="129"/>
-      <c r="E28" s="129"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="133"/>
       <c r="F28" s="32">
         <v>1.5</v>
       </c>
@@ -10180,11 +10181,11 @@
       <c r="B29" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="129" t="s">
+      <c r="C29" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="129"/>
-      <c r="E29" s="129"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="133"/>
       <c r="F29" s="32">
         <v>0.5</v>
       </c>
@@ -10197,11 +10198,11 @@
       <c r="B30" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="129" t="s">
+      <c r="C30" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="129"/>
-      <c r="E30" s="129"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="133"/>
       <c r="F30" s="32">
         <v>1</v>
       </c>
@@ -10214,11 +10215,11 @@
       <c r="B31" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="129" t="s">
+      <c r="C31" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="129"/>
-      <c r="E31" s="129"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
       <c r="F31" s="32">
         <v>0.5</v>
       </c>
@@ -10231,11 +10232,11 @@
       <c r="B32" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="129" t="s">
+      <c r="C32" s="133" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="129"/>
-      <c r="E32" s="129"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="133"/>
       <c r="F32" s="32">
         <v>1</v>
       </c>
@@ -10248,11 +10249,11 @@
       <c r="B33" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="129" t="s">
+      <c r="C33" s="133" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="129"/>
-      <c r="E33" s="129"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="133"/>
       <c r="F33" s="32">
         <v>2</v>
       </c>
@@ -10265,11 +10266,11 @@
       <c r="B34" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="129" t="s">
+      <c r="C34" s="133" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="129"/>
-      <c r="E34" s="129"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="133"/>
       <c r="F34" s="32">
         <v>-1</v>
       </c>
@@ -10282,11 +10283,11 @@
       <c r="B35" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="129" t="s">
+      <c r="C35" s="133" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="129"/>
-      <c r="E35" s="129"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
       <c r="F35" s="32">
         <v>-1</v>
       </c>
@@ -10312,11 +10313,6 @@
   </sheetData>
   <sheetProtection password="C6D5" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="14">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
@@ -10326,13 +10322,18 @@
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21">
+    <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G28:G35 I28:I35">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G28:G35 I28:I35" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
@@ -10343,7 +10344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>

</xml_diff>